<commit_message>
advanced import excel data
</commit_message>
<xml_diff>
--- a/public/excel/template_cfdi_import.xlsx
+++ b/public/excel/template_cfdi_import.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29122"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29203"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{92727D65-C3A4-441D-8D40-0C7D5AD2BB44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2C18D510-38CD-43A2-9E9A-ACABC4B3806E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="50">
   <si>
     <t>tipo</t>
   </si>
@@ -105,6 +105,9 @@
     <t>impuesto</t>
   </si>
   <si>
+    <t>obj_imp</t>
+  </si>
+  <si>
     <t>cfdi</t>
   </si>
   <si>
@@ -159,7 +162,13 @@
     <t>IVA</t>
   </si>
   <si>
+    <t>01</t>
+  </si>
+  <si>
     <t>Exento</t>
+  </si>
+  <si>
+    <t>02</t>
   </si>
   <si>
     <t>xxxxx</t>
@@ -178,7 +187,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -206,6 +215,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -215,7 +232,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -238,16 +255,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -582,10 +615,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X8"/>
+  <dimension ref="A1:Y9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="Y9" sqref="Y9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -607,7 +640,7 @@
     <col min="24" max="24" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -677,46 +710,49 @@
       <c r="W1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="X1" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="Y1" s="3" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="2" spans="1:24">
+    <row r="2" spans="1:25">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H2">
         <v>42501</v>
       </c>
       <c r="I2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="J2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="K2">
         <v>1</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="M2">
         <v>55</v>
@@ -725,30 +761,31 @@
         <v>55</v>
       </c>
       <c r="O2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="P2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="Q2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="R2" t="s">
-        <v>37</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="Y2" s="6"/>
     </row>
-    <row r="3" spans="1:24">
+    <row r="3" spans="1:25">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="U3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="V3" s="2">
         <v>1010101</v>
@@ -757,21 +794,24 @@
         <v>20</v>
       </c>
       <c r="X3" t="s">
-        <v>41</v>
+        <v>42</v>
+      </c>
+      <c r="Y3" s="6" t="s">
+        <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:24">
+    <row r="4" spans="1:25">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="S4">
         <v>3</v>
       </c>
       <c r="T4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="U4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="V4" s="2">
         <v>1010101</v>
@@ -780,45 +820,48 @@
         <v>15</v>
       </c>
       <c r="X4" t="s">
-        <v>42</v>
+        <v>44</v>
+      </c>
+      <c r="Y4" s="6" t="s">
+        <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:24">
+    <row r="5" spans="1:25">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C5" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H5">
         <v>42501</v>
       </c>
       <c r="I5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="J5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="K5">
         <v>2</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="M5">
         <v>10</v>
@@ -827,30 +870,31 @@
         <v>10</v>
       </c>
       <c r="O5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="P5" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="Q5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="R5" t="s">
-        <v>37</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="Y5" s="6"/>
     </row>
-    <row r="6" spans="1:24">
+    <row r="6" spans="1:25">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="S6">
         <v>1</v>
       </c>
       <c r="T6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="U6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="V6" s="2">
         <v>1010101</v>
@@ -859,45 +903,48 @@
         <v>10</v>
       </c>
       <c r="X6" t="s">
-        <v>41</v>
+        <v>42</v>
+      </c>
+      <c r="Y6" s="6" t="s">
+        <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:24">
+    <row r="7" spans="1:25">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" t="s">
         <v>29</v>
       </c>
-      <c r="D7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
+        <v>46</v>
+      </c>
+      <c r="G7" t="s">
         <v>28</v>
-      </c>
-      <c r="F7" t="s">
-        <v>43</v>
-      </c>
-      <c r="G7" t="s">
-        <v>27</v>
       </c>
       <c r="H7">
         <v>42501</v>
       </c>
       <c r="I7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="J7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="K7">
         <v>3</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="M7">
         <v>15</v>
@@ -906,30 +953,31 @@
         <v>15</v>
       </c>
       <c r="O7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="P7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="Q7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="R7" t="s">
-        <v>37</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="Y7" s="6"/>
     </row>
-    <row r="8" spans="1:24">
+    <row r="8" spans="1:25">
       <c r="A8" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="S8">
         <v>1</v>
       </c>
       <c r="T8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="U8" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="V8" s="2">
         <v>1010101</v>
@@ -938,8 +986,14 @@
         <v>15</v>
       </c>
       <c r="X8" t="s">
-        <v>41</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="Y8" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25">
+      <c r="Y9" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>